<commit_message>
Updated Vr/models/Unity/Asset List/ Calendar
</commit_message>
<xml_diff>
--- a/Schedule/Asset List:Schedule.xlsx
+++ b/Schedule/Asset List:Schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corbinwalker/Documents/Digital Media/DGM-3650/Asset List:"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corbinwalker/Documents/Digital Media/DGM-3650/Schedule/Asset List:"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9409F4FF-BDF0-0347-B832-F5F74736DE44}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{057E2320-DA64-7444-B858-A57D9B288112}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="460" windowWidth="27820" windowHeight="17040" activeTab="1" xr2:uid="{8439A946-5B6C-3D45-A729-A84689364E52}"/>
+    <workbookView xWindow="600" yWindow="460" windowWidth="27820" windowHeight="17040" xr2:uid="{8439A946-5B6C-3D45-A729-A84689364E52}"/>
   </bookViews>
   <sheets>
     <sheet name="Assest List" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="78">
   <si>
     <t>Asset List</t>
   </si>
@@ -35,33 +35,18 @@
     <t>Models</t>
   </si>
   <si>
-    <t>Scripting</t>
-  </si>
-  <si>
-    <t>Sounds</t>
-  </si>
-  <si>
     <t>History/Resources</t>
   </si>
   <si>
     <t>Enviroment</t>
   </si>
   <si>
-    <t>Special Effects</t>
-  </si>
-  <si>
     <t>Resources Needed</t>
   </si>
   <si>
     <t>Statue of Athena</t>
   </si>
   <si>
-    <t>Statues Front Entrance</t>
-  </si>
-  <si>
-    <t>Statues Back Entrance</t>
-  </si>
-  <si>
     <t>Script</t>
   </si>
   <si>
@@ -74,39 +59,6 @@
     <t>UV Maps</t>
   </si>
   <si>
-    <t>Main Page UI</t>
-  </si>
-  <si>
-    <t>Camera Movement coding</t>
-  </si>
-  <si>
-    <t>Information UI</t>
-  </si>
-  <si>
-    <t>Sound UI</t>
-  </si>
-  <si>
-    <t>Breeze</t>
-  </si>
-  <si>
-    <t>Fire crakling</t>
-  </si>
-  <si>
-    <t>Daytime noise</t>
-  </si>
-  <si>
-    <t>Night Time Noise</t>
-  </si>
-  <si>
-    <t>Dust falling</t>
-  </si>
-  <si>
-    <t>Bird Chirpping</t>
-  </si>
-  <si>
-    <t>Wind</t>
-  </si>
-  <si>
     <t>History/ Resources</t>
   </si>
   <si>
@@ -143,27 +95,6 @@
     <t xml:space="preserve">Date Expected </t>
   </si>
   <si>
-    <t>Clouds</t>
-  </si>
-  <si>
-    <t>Lighting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fire </t>
-  </si>
-  <si>
-    <t>Rain</t>
-  </si>
-  <si>
-    <t>Thunder/Lightning</t>
-  </si>
-  <si>
-    <t>Scrolling UI</t>
-  </si>
-  <si>
-    <t>Lightning</t>
-  </si>
-  <si>
     <t>Schedule</t>
   </si>
   <si>
@@ -239,9 +170,6 @@
     <t>Oct 18, 2018</t>
   </si>
   <si>
-    <t>Oct 11,2018</t>
-  </si>
-  <si>
     <t>November</t>
   </si>
   <si>
@@ -254,18 +182,9 @@
     <t>Oct 25, 2018</t>
   </si>
   <si>
-    <t>Nov 04, 2018</t>
-  </si>
-  <si>
     <t>Nov 11, 2018</t>
   </si>
   <si>
-    <t>Nov 18, 2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Special Effects </t>
-  </si>
-  <si>
     <t>Enviorments/ Special</t>
   </si>
   <si>
@@ -278,12 +197,6 @@
     <t>Nov 25, 2018</t>
   </si>
   <si>
-    <t>Statues for both Entrance</t>
-  </si>
-  <si>
-    <t>and back completed</t>
-  </si>
-  <si>
     <t>End of the semester</t>
   </si>
   <si>
@@ -296,16 +209,58 @@
     <t>Statue of Athena WB</t>
   </si>
   <si>
-    <t>put into VR and Also</t>
-  </si>
-  <si>
-    <t>scaled in Vr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">simple Ui created for </t>
-  </si>
-  <si>
-    <t>Play testing</t>
+    <t>VR</t>
+  </si>
+  <si>
+    <t>Getting the models into</t>
+  </si>
+  <si>
+    <t>Unity</t>
+  </si>
+  <si>
+    <t>Getting VR to Work</t>
+  </si>
+  <si>
+    <t>Getting the models to</t>
+  </si>
+  <si>
+    <t>Scale</t>
+  </si>
+  <si>
+    <t>Models WB</t>
+  </si>
+  <si>
+    <t>Nov 16, 2018</t>
+  </si>
+  <si>
+    <t>Dec 1, 2018</t>
+  </si>
+  <si>
+    <t>Nov 16,2018</t>
+  </si>
+  <si>
+    <t>Nov 20,2018</t>
+  </si>
+  <si>
+    <t>Oct 5, 2018</t>
+  </si>
+  <si>
+    <t>Oct 10, 2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">put into VR </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get Scaled Correctly for </t>
+  </si>
+  <si>
+    <t>Oct 11, 2018</t>
+  </si>
+  <si>
+    <t>Nov 4, 2018</t>
+  </si>
+  <si>
+    <t>completed / VR to work</t>
   </si>
 </sst>
 </file>
@@ -566,35 +521,35 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp10.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp11.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp13.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp14.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp15.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp16.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp17.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp18.xml><?xml version="1.0" encoding="utf-8"?>
@@ -602,19 +557,19 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp19.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp20.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp21.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp22.xml><?xml version="1.0" encoding="utf-8"?>
@@ -622,74 +577,14 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp23.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp24.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp25.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp26.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp27.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp28.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp29.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp30.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp31.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp32.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp33.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp34.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp35.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp36.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp37.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp38.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp39.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
 </file>
 
@@ -702,11 +597,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp8.xml><?xml version="1.0" encoding="utf-8"?>
@@ -993,73 +888,6 @@
         <xdr:from>
           <xdr:col>13</xdr:col>
           <xdr:colOff>228600</xdr:colOff>
-          <xdr:row>6</xdr:row>
-          <xdr:rowOff>114300</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>13</xdr:col>
-          <xdr:colOff>584200</xdr:colOff>
-          <xdr:row>8</xdr:row>
-          <xdr:rowOff>12700</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1032" name="Check Box 8" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1032"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008040000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>13</xdr:col>
-          <xdr:colOff>228600</xdr:colOff>
           <xdr:row>7</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
@@ -1127,13 +955,13 @@
         <xdr:from>
           <xdr:col>13</xdr:col>
           <xdr:colOff>228600</xdr:colOff>
-          <xdr:row>9</xdr:row>
+          <xdr:row>7</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>13</xdr:col>
           <xdr:colOff>584200</xdr:colOff>
-          <xdr:row>11</xdr:row>
+          <xdr:row>9</xdr:row>
           <xdr:rowOff>12700</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -1194,13 +1022,13 @@
         <xdr:from>
           <xdr:col>13</xdr:col>
           <xdr:colOff>228600</xdr:colOff>
-          <xdr:row>10</xdr:row>
+          <xdr:row>8</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>13</xdr:col>
           <xdr:colOff>584200</xdr:colOff>
-          <xdr:row>12</xdr:row>
+          <xdr:row>10</xdr:row>
           <xdr:rowOff>12700</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -1261,13 +1089,13 @@
         <xdr:from>
           <xdr:col>13</xdr:col>
           <xdr:colOff>228600</xdr:colOff>
-          <xdr:row>11</xdr:row>
+          <xdr:row>9</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>13</xdr:col>
           <xdr:colOff>584200</xdr:colOff>
-          <xdr:row>13</xdr:row>
+          <xdr:row>11</xdr:row>
           <xdr:rowOff>12700</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -1328,24 +1156,91 @@
         <xdr:from>
           <xdr:col>13</xdr:col>
           <xdr:colOff>228600</xdr:colOff>
-          <xdr:row>12</xdr:row>
+          <xdr:row>11</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>13</xdr:col>
           <xdr:colOff>584200</xdr:colOff>
-          <xdr:row>14</xdr:row>
+          <xdr:row>13</xdr:row>
           <xdr:rowOff>12700</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1037" name="Check Box 13" hidden="1">
+            <xdr:cNvPr id="1038" name="Check Box 14" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1037"/>
+                  <a14:compatExt spid="_x0000_s1038"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>13</xdr:col>
+          <xdr:colOff>228600</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>114300</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>13</xdr:col>
+          <xdr:colOff>584200</xdr:colOff>
+          <xdr:row>13</xdr:row>
+          <xdr:rowOff>12700</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1039" name="Check Box 15" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1039"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1406,13 +1301,13 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1038" name="Check Box 14" hidden="1">
+            <xdr:cNvPr id="1041" name="Check Box 17" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1038"/>
+                  <a14:compatExt spid="_x0000_s1041"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000011040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1462,91 +1357,24 @@
         <xdr:from>
           <xdr:col>13</xdr:col>
           <xdr:colOff>228600</xdr:colOff>
-          <xdr:row>15</xdr:row>
+          <xdr:row>14</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>13</xdr:col>
           <xdr:colOff>584200</xdr:colOff>
-          <xdr:row>17</xdr:row>
+          <xdr:row>16</xdr:row>
           <xdr:rowOff>12700</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1039" name="Check Box 15" hidden="1">
+            <xdr:cNvPr id="1042" name="Check Box 18" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1039"/>
+                  <a14:compatExt spid="_x0000_s1042"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F040000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>13</xdr:col>
-          <xdr:colOff>228600</xdr:colOff>
-          <xdr:row>16</xdr:row>
-          <xdr:rowOff>114300</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>13</xdr:col>
-          <xdr:colOff>584200</xdr:colOff>
-          <xdr:row>18</xdr:row>
-          <xdr:rowOff>12700</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1040" name="Check Box 16" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1040"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000010040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000012040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1607,13 +1435,13 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1041" name="Check Box 17" hidden="1">
+            <xdr:cNvPr id="1052" name="Check Box 28" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1041"/>
+                  <a14:compatExt spid="_x0000_s1052"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000011040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001C040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1674,13 +1502,13 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1042" name="Check Box 18" hidden="1">
+            <xdr:cNvPr id="1053" name="Check Box 29" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1042"/>
+                  <a14:compatExt spid="_x0000_s1053"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000012040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001D040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1741,13 +1569,80 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1043" name="Check Box 19" hidden="1">
+            <xdr:cNvPr id="1054" name="Check Box 30" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1043"/>
+                  <a14:compatExt spid="_x0000_s1054"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000013040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001E040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>13</xdr:col>
+          <xdr:colOff>228600</xdr:colOff>
+          <xdr:row>20</xdr:row>
+          <xdr:rowOff>114300</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>13</xdr:col>
+          <xdr:colOff>584200</xdr:colOff>
+          <xdr:row>22</xdr:row>
+          <xdr:rowOff>12700</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1055" name="Check Box 31" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1055"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001F040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1808,80 +1703,13 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1044" name="Check Box 20" hidden="1">
+            <xdr:cNvPr id="1056" name="Check Box 32" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1044"/>
+                  <a14:compatExt spid="_x0000_s1056"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000014040000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>13</xdr:col>
-          <xdr:colOff>228600</xdr:colOff>
-          <xdr:row>22</xdr:row>
-          <xdr:rowOff>114300</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>13</xdr:col>
-          <xdr:colOff>584200</xdr:colOff>
-          <xdr:row>24</xdr:row>
-          <xdr:rowOff>12700</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1045" name="Check Box 21" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1045"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000015040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000020040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1942,13 +1770,13 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1046" name="Check Box 22" hidden="1">
+            <xdr:cNvPr id="1057" name="Check Box 33" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1046"/>
+                  <a14:compatExt spid="_x0000_s1057"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000016040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000021040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2009,13 +1837,13 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1047" name="Check Box 23" hidden="1">
+            <xdr:cNvPr id="1058" name="Check Box 34" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1047"/>
+                  <a14:compatExt spid="_x0000_s1058"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000017040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000022040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2076,13 +1904,13 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1048" name="Check Box 24" hidden="1">
+            <xdr:cNvPr id="1059" name="Check Box 35" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1048"/>
+                  <a14:compatExt spid="_x0000_s1059"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2143,743 +1971,6 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1049" name="Check Box 25" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1049"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000019040000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>13</xdr:col>
-          <xdr:colOff>228600</xdr:colOff>
-          <xdr:row>27</xdr:row>
-          <xdr:rowOff>114300</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>13</xdr:col>
-          <xdr:colOff>584200</xdr:colOff>
-          <xdr:row>29</xdr:row>
-          <xdr:rowOff>12700</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1050" name="Check Box 26" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1050"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001A040000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>13</xdr:col>
-          <xdr:colOff>228600</xdr:colOff>
-          <xdr:row>28</xdr:row>
-          <xdr:rowOff>114300</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>13</xdr:col>
-          <xdr:colOff>584200</xdr:colOff>
-          <xdr:row>30</xdr:row>
-          <xdr:rowOff>12700</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1051" name="Check Box 27" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1051"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001B040000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>13</xdr:col>
-          <xdr:colOff>228600</xdr:colOff>
-          <xdr:row>30</xdr:row>
-          <xdr:rowOff>114300</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>13</xdr:col>
-          <xdr:colOff>584200</xdr:colOff>
-          <xdr:row>32</xdr:row>
-          <xdr:rowOff>12700</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1052" name="Check Box 28" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1052"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001C040000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>13</xdr:col>
-          <xdr:colOff>228600</xdr:colOff>
-          <xdr:row>31</xdr:row>
-          <xdr:rowOff>114300</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>13</xdr:col>
-          <xdr:colOff>584200</xdr:colOff>
-          <xdr:row>33</xdr:row>
-          <xdr:rowOff>12700</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1053" name="Check Box 29" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1053"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001D040000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>13</xdr:col>
-          <xdr:colOff>228600</xdr:colOff>
-          <xdr:row>32</xdr:row>
-          <xdr:rowOff>114300</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>13</xdr:col>
-          <xdr:colOff>584200</xdr:colOff>
-          <xdr:row>34</xdr:row>
-          <xdr:rowOff>12700</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1054" name="Check Box 30" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1054"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001E040000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>13</xdr:col>
-          <xdr:colOff>228600</xdr:colOff>
-          <xdr:row>33</xdr:row>
-          <xdr:rowOff>114300</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>13</xdr:col>
-          <xdr:colOff>584200</xdr:colOff>
-          <xdr:row>35</xdr:row>
-          <xdr:rowOff>12700</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1055" name="Check Box 31" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1055"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001F040000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>13</xdr:col>
-          <xdr:colOff>228600</xdr:colOff>
-          <xdr:row>34</xdr:row>
-          <xdr:rowOff>114300</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>13</xdr:col>
-          <xdr:colOff>584200</xdr:colOff>
-          <xdr:row>36</xdr:row>
-          <xdr:rowOff>12700</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1056" name="Check Box 32" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1056"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000020040000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>13</xdr:col>
-          <xdr:colOff>228600</xdr:colOff>
-          <xdr:row>36</xdr:row>
-          <xdr:rowOff>114300</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>13</xdr:col>
-          <xdr:colOff>584200</xdr:colOff>
-          <xdr:row>38</xdr:row>
-          <xdr:rowOff>12700</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1057" name="Check Box 33" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1057"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000021040000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>13</xdr:col>
-          <xdr:colOff>228600</xdr:colOff>
-          <xdr:row>37</xdr:row>
-          <xdr:rowOff>114300</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>13</xdr:col>
-          <xdr:colOff>584200</xdr:colOff>
-          <xdr:row>39</xdr:row>
-          <xdr:rowOff>12700</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1058" name="Check Box 34" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1058"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000022040000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>13</xdr:col>
-          <xdr:colOff>228600</xdr:colOff>
-          <xdr:row>38</xdr:row>
-          <xdr:rowOff>114300</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>13</xdr:col>
-          <xdr:colOff>584200</xdr:colOff>
-          <xdr:row>40</xdr:row>
-          <xdr:rowOff>12700</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1059" name="Check Box 35" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1059"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023040000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>13</xdr:col>
-          <xdr:colOff>228600</xdr:colOff>
-          <xdr:row>39</xdr:row>
-          <xdr:rowOff>114300</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>13</xdr:col>
-          <xdr:colOff>584200</xdr:colOff>
-          <xdr:row>41</xdr:row>
-          <xdr:rowOff>12700</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
             <xdr:cNvPr id="1060" name="Check Box 36" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
@@ -2887,341 +1978,6 @@
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
                   <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000024040000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>13</xdr:col>
-          <xdr:colOff>228600</xdr:colOff>
-          <xdr:row>40</xdr:row>
-          <xdr:rowOff>114300</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>13</xdr:col>
-          <xdr:colOff>584200</xdr:colOff>
-          <xdr:row>42</xdr:row>
-          <xdr:rowOff>12700</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1061" name="Check Box 37" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1061"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000025040000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>13</xdr:col>
-          <xdr:colOff>228600</xdr:colOff>
-          <xdr:row>42</xdr:row>
-          <xdr:rowOff>114300</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>13</xdr:col>
-          <xdr:colOff>584200</xdr:colOff>
-          <xdr:row>44</xdr:row>
-          <xdr:rowOff>12700</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1062" name="Check Box 38" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1062"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000026040000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>13</xdr:col>
-          <xdr:colOff>228600</xdr:colOff>
-          <xdr:row>43</xdr:row>
-          <xdr:rowOff>114300</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>13</xdr:col>
-          <xdr:colOff>584200</xdr:colOff>
-          <xdr:row>45</xdr:row>
-          <xdr:rowOff>12700</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1063" name="Check Box 39" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1063"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000027040000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>13</xdr:col>
-          <xdr:colOff>228600</xdr:colOff>
-          <xdr:row>44</xdr:row>
-          <xdr:rowOff>114300</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>13</xdr:col>
-          <xdr:colOff>584200</xdr:colOff>
-          <xdr:row>46</xdr:row>
-          <xdr:rowOff>12700</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1064" name="Check Box 40" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1064"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000028040000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>13</xdr:col>
-          <xdr:colOff>228600</xdr:colOff>
-          <xdr:row>45</xdr:row>
-          <xdr:rowOff>114300</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>13</xdr:col>
-          <xdr:colOff>584200</xdr:colOff>
-          <xdr:row>47</xdr:row>
-          <xdr:rowOff>12700</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1065" name="Check Box 41" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1065"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000029040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3329,6 +2085,130 @@
         </xdr:sp>
         <xdr:clientData/>
       </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>13</xdr:col>
+          <xdr:colOff>228600</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>114300</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="355600" cy="304800"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1067" name="Check Box 43" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1067"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E56DF9EC-B4A9-624A-BF24-06DEC30257E2}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>13</xdr:col>
+          <xdr:colOff>228600</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>114300</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="355600" cy="304800"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1068" name="Check Box 44" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1068"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7A6AB09-212C-1A43-9B41-B16F543571E5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
@@ -3632,10 +2512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C482110C-7707-D04A-B6A5-4E040EFC0030}">
-  <dimension ref="A1:AD47"/>
+  <dimension ref="A1:AD29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3652,39 +2532,39 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="M2" s="1"/>
       <c r="N2" s="1" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="O2" s="1"/>
       <c r="P2" s="1" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="Q2" s="1"/>
       <c r="R2" s="1" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="S2" s="1"/>
       <c r="T2" s="1" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="U2" s="1"/>
       <c r="V2" s="1" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
@@ -3697,7 +2577,7 @@
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -3742,7 +2622,7 @@
       <c r="P4" s="6"/>
       <c r="R4" s="6"/>
       <c r="T4" s="8" t="s">
-        <v>73</v>
+        <v>49</v>
       </c>
       <c r="V4" s="6"/>
       <c r="W4" s="6"/>
@@ -3755,8 +2635,8 @@
       <c r="AD4" s="6"/>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B5" s="4" t="s">
-        <v>2</v>
+      <c r="B5" s="5" t="s">
+        <v>60</v>
       </c>
       <c r="C5" s="4"/>
       <c r="F5" s="6"/>
@@ -3764,10 +2644,12 @@
       <c r="J5" s="6"/>
       <c r="L5" s="6"/>
       <c r="N5" s="6"/>
-      <c r="P5" s="6"/>
+      <c r="P5" s="9" t="s">
+        <v>70</v>
+      </c>
       <c r="R5" s="6"/>
       <c r="T5" s="8" t="s">
-        <v>73</v>
+        <v>49</v>
       </c>
       <c r="V5" s="6"/>
       <c r="W5" s="6"/>
@@ -3781,7 +2663,7 @@
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6" s="4"/>
       <c r="F6" s="6"/>
@@ -3789,24 +2671,17 @@
       <c r="J6" s="6"/>
       <c r="L6" s="6"/>
       <c r="N6" s="6"/>
-      <c r="P6" s="6"/>
+      <c r="P6" s="9" t="s">
+        <v>25</v>
+      </c>
       <c r="R6" s="6"/>
       <c r="T6" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="V6" s="6"/>
-      <c r="W6" s="6"/>
-      <c r="X6" s="6"/>
-      <c r="Y6" s="6"/>
-      <c r="Z6" s="6"/>
-      <c r="AA6" s="6"/>
-      <c r="AB6" s="6"/>
-      <c r="AC6" s="6"/>
-      <c r="AD6" s="6"/>
+        <v>25</v>
+      </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B7" s="4" t="s">
-        <v>4</v>
+      <c r="B7" s="5" t="s">
+        <v>3</v>
       </c>
       <c r="C7" s="4"/>
       <c r="F7" s="6"/>
@@ -3817,7 +2692,7 @@
       <c r="P7" s="6"/>
       <c r="R7" s="6"/>
       <c r="T7" s="8" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="V7" s="6"/>
       <c r="W7" s="6"/>
@@ -3830,33 +2705,42 @@
       <c r="AD7" s="6"/>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="4"/>
-      <c r="F8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="N8" s="6"/>
-      <c r="P8" s="6"/>
-      <c r="R8" s="6"/>
-      <c r="T8" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="V8" s="6"/>
-      <c r="W8" s="6"/>
-      <c r="X8" s="6"/>
-      <c r="Y8" s="6"/>
-      <c r="Z8" s="6"/>
-      <c r="AA8" s="6"/>
-      <c r="AB8" s="6"/>
-      <c r="AC8" s="6"/>
-      <c r="AD8" s="6"/>
+      <c r="A8" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="2"/>
+      <c r="Y8" s="2"/>
+      <c r="Z8" s="2"/>
+      <c r="AA8" s="2"/>
+      <c r="AB8" s="2"/>
+      <c r="AC8" s="2"/>
+      <c r="AD8" s="2"/>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B9" s="4" t="s">
-        <v>6</v>
+      <c r="B9" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="C9" s="4"/>
       <c r="F9" s="6"/>
@@ -3864,10 +2748,12 @@
       <c r="J9" s="6"/>
       <c r="L9" s="6"/>
       <c r="N9" s="6"/>
-      <c r="P9" s="6"/>
+      <c r="P9" s="9" t="s">
+        <v>71</v>
+      </c>
       <c r="R9" s="6"/>
-      <c r="T9" s="8" t="s">
-        <v>73</v>
+      <c r="T9" s="9" t="s">
+        <v>46</v>
       </c>
       <c r="V9" s="6"/>
       <c r="W9" s="6"/>
@@ -3880,42 +2766,35 @@
       <c r="AD9" s="6"/>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
-      <c r="R10" s="2"/>
-      <c r="S10" s="2"/>
-      <c r="T10" s="2"/>
-      <c r="U10" s="2"/>
-      <c r="V10" s="2"/>
-      <c r="W10" s="2"/>
-      <c r="X10" s="2"/>
-      <c r="Y10" s="2"/>
-      <c r="Z10" s="2"/>
-      <c r="AA10" s="2"/>
-      <c r="AB10" s="2"/>
-      <c r="AC10" s="2"/>
-      <c r="AD10" s="2"/>
+      <c r="B10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="F10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="P10" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="R10" s="6"/>
+      <c r="T10" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="V10" s="6"/>
+      <c r="W10" s="6"/>
+      <c r="X10" s="6"/>
+      <c r="Y10" s="6"/>
+      <c r="Z10" s="6"/>
+      <c r="AA10" s="6"/>
+      <c r="AB10" s="6"/>
+      <c r="AC10" s="6"/>
+      <c r="AD10" s="6"/>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B11" s="5" t="s">
-        <v>54</v>
+      <c r="B11" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="C11" s="4"/>
       <c r="F11" s="6"/>
@@ -3926,7 +2805,7 @@
       <c r="P11" s="6"/>
       <c r="R11" s="6"/>
       <c r="T11" s="9" t="s">
-        <v>76</v>
+        <v>50</v>
       </c>
       <c r="V11" s="6"/>
       <c r="W11" s="6"/>
@@ -3939,33 +2818,42 @@
       <c r="AD11" s="6"/>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B12" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C12" s="4"/>
-      <c r="F12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="N12" s="6"/>
-      <c r="P12" s="6"/>
-      <c r="R12" s="6"/>
-      <c r="T12" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="V12" s="6"/>
-      <c r="W12" s="6"/>
-      <c r="X12" s="6"/>
-      <c r="Y12" s="6"/>
-      <c r="Z12" s="6"/>
-      <c r="AA12" s="6"/>
-      <c r="AB12" s="6"/>
-      <c r="AC12" s="6"/>
-      <c r="AD12" s="6"/>
+      <c r="A12" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2"/>
+      <c r="V12" s="2"/>
+      <c r="W12" s="2"/>
+      <c r="X12" s="2"/>
+      <c r="Y12" s="2"/>
+      <c r="Z12" s="2"/>
+      <c r="AA12" s="2"/>
+      <c r="AB12" s="2"/>
+      <c r="AC12" s="2"/>
+      <c r="AD12" s="2"/>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B13" s="4" t="s">
-        <v>8</v>
+      <c r="B13" s="5" t="s">
+        <v>61</v>
       </c>
       <c r="C13" s="4"/>
       <c r="F13" s="6"/>
@@ -3973,10 +2861,12 @@
       <c r="J13" s="6"/>
       <c r="L13" s="6"/>
       <c r="N13" s="6"/>
-      <c r="P13" s="6"/>
+      <c r="P13" s="9" t="s">
+        <v>69</v>
+      </c>
       <c r="R13" s="6"/>
       <c r="T13" s="9" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="V13" s="6"/>
       <c r="W13" s="6"/>
@@ -3990,7 +2880,7 @@
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B14" s="5" t="s">
-        <v>9</v>
+        <v>62</v>
       </c>
       <c r="C14" s="4"/>
       <c r="F14" s="6"/>
@@ -4000,9 +2890,7 @@
       <c r="N14" s="6"/>
       <c r="P14" s="6"/>
       <c r="R14" s="6"/>
-      <c r="T14" s="9" t="s">
-        <v>77</v>
-      </c>
+      <c r="T14" s="9"/>
       <c r="V14" s="6"/>
       <c r="W14" s="6"/>
       <c r="X14" s="6"/>
@@ -4015,7 +2903,7 @@
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B15" s="5" t="s">
-        <v>10</v>
+        <v>63</v>
       </c>
       <c r="C15" s="4"/>
       <c r="F15" s="6"/>
@@ -4023,10 +2911,12 @@
       <c r="J15" s="6"/>
       <c r="L15" s="6"/>
       <c r="N15" s="6"/>
-      <c r="P15" s="6"/>
+      <c r="P15" s="9" t="s">
+        <v>69</v>
+      </c>
       <c r="R15" s="6"/>
       <c r="T15" s="9" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="V15" s="6"/>
       <c r="W15" s="6"/>
@@ -4039,42 +2929,35 @@
       <c r="AD15" s="6"/>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
-      <c r="P16" s="2"/>
-      <c r="Q16" s="2"/>
-      <c r="R16" s="2"/>
-      <c r="S16" s="2"/>
-      <c r="T16" s="2"/>
-      <c r="U16" s="2"/>
-      <c r="V16" s="2"/>
-      <c r="W16" s="2"/>
-      <c r="X16" s="2"/>
-      <c r="Y16" s="2"/>
-      <c r="Z16" s="2"/>
-      <c r="AA16" s="2"/>
-      <c r="AB16" s="2"/>
-      <c r="AC16" s="2"/>
-      <c r="AD16" s="2"/>
+      <c r="B16" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" s="4"/>
+      <c r="F16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="P16" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="R16" s="6"/>
+      <c r="T16" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="V16" s="6"/>
+      <c r="W16" s="6"/>
+      <c r="X16" s="6"/>
+      <c r="Y16" s="6"/>
+      <c r="Z16" s="6"/>
+      <c r="AA16" s="6"/>
+      <c r="AB16" s="6"/>
+      <c r="AC16" s="6"/>
+      <c r="AD16" s="6"/>
     </row>
     <row r="17" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B17" s="5" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="C17" s="4"/>
       <c r="F17" s="6"/>
@@ -4084,9 +2967,7 @@
       <c r="N17" s="6"/>
       <c r="P17" s="6"/>
       <c r="R17" s="6"/>
-      <c r="T17" s="9" t="s">
-        <v>69</v>
-      </c>
+      <c r="T17" s="9"/>
       <c r="V17" s="6"/>
       <c r="W17" s="6"/>
       <c r="X17" s="6"/>
@@ -4098,33 +2979,42 @@
       <c r="AD17" s="6"/>
     </row>
     <row r="18" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B18" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="4"/>
-      <c r="F18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="L18" s="6"/>
-      <c r="N18" s="6"/>
-      <c r="P18" s="6"/>
-      <c r="R18" s="6"/>
-      <c r="T18" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="V18" s="6"/>
-      <c r="W18" s="6"/>
-      <c r="X18" s="6"/>
-      <c r="Y18" s="6"/>
-      <c r="Z18" s="6"/>
-      <c r="AA18" s="6"/>
-      <c r="AB18" s="6"/>
-      <c r="AC18" s="6"/>
-      <c r="AD18" s="6"/>
+      <c r="A18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+      <c r="S18" s="2"/>
+      <c r="T18" s="2"/>
+      <c r="U18" s="2"/>
+      <c r="V18" s="2"/>
+      <c r="W18" s="2"/>
+      <c r="X18" s="2"/>
+      <c r="Y18" s="2"/>
+      <c r="Z18" s="2"/>
+      <c r="AA18" s="2"/>
+      <c r="AB18" s="2"/>
+      <c r="AC18" s="2"/>
+      <c r="AD18" s="2"/>
     </row>
     <row r="19" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B19" s="5" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="C19" s="4"/>
       <c r="F19" s="6"/>
@@ -4132,10 +3022,12 @@
       <c r="J19" s="6"/>
       <c r="L19" s="6"/>
       <c r="N19" s="6"/>
-      <c r="P19" s="6"/>
+      <c r="P19" s="9" t="s">
+        <v>25</v>
+      </c>
       <c r="R19" s="6"/>
       <c r="T19" s="9" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="V19" s="6"/>
       <c r="W19" s="6"/>
@@ -4149,7 +3041,7 @@
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B20" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C20" s="4"/>
       <c r="F20" s="6"/>
@@ -4157,10 +3049,12 @@
       <c r="J20" s="6"/>
       <c r="L20" s="6"/>
       <c r="N20" s="6"/>
-      <c r="P20" s="6"/>
+      <c r="P20" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="R20" s="6"/>
       <c r="T20" s="9" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="V20" s="6"/>
       <c r="W20" s="6"/>
@@ -4174,7 +3068,7 @@
     </row>
     <row r="21" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B21" s="5" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="C21" s="4"/>
       <c r="F21" s="6"/>
@@ -4182,10 +3076,12 @@
       <c r="J21" s="6"/>
       <c r="L21" s="6"/>
       <c r="N21" s="6"/>
-      <c r="P21" s="6"/>
+      <c r="P21" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="R21" s="6"/>
       <c r="T21" s="9" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="V21" s="6"/>
       <c r="W21" s="6"/>
@@ -4198,42 +3094,35 @@
       <c r="AD21" s="6"/>
     </row>
     <row r="22" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
-      <c r="O22" s="2"/>
-      <c r="P22" s="2"/>
-      <c r="Q22" s="2"/>
-      <c r="R22" s="2"/>
-      <c r="S22" s="2"/>
-      <c r="T22" s="2"/>
-      <c r="U22" s="2"/>
-      <c r="V22" s="2"/>
-      <c r="W22" s="2"/>
-      <c r="X22" s="2"/>
-      <c r="Y22" s="2"/>
-      <c r="Z22" s="2"/>
-      <c r="AA22" s="2"/>
-      <c r="AB22" s="2"/>
-      <c r="AC22" s="2"/>
-      <c r="AD22" s="2"/>
+      <c r="B22" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="4"/>
+      <c r="F22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="N22" s="6"/>
+      <c r="P22" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="R22" s="6"/>
+      <c r="T22" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="V22" s="6"/>
+      <c r="W22" s="6"/>
+      <c r="X22" s="6"/>
+      <c r="Y22" s="6"/>
+      <c r="Z22" s="6"/>
+      <c r="AA22" s="6"/>
+      <c r="AB22" s="6"/>
+      <c r="AC22" s="6"/>
+      <c r="AD22" s="6"/>
     </row>
     <row r="23" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B23" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C23" s="4"/>
       <c r="F23" s="6"/>
@@ -4241,10 +3130,12 @@
       <c r="J23" s="6"/>
       <c r="L23" s="6"/>
       <c r="N23" s="6"/>
-      <c r="P23" s="6"/>
+      <c r="P23" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="R23" s="6"/>
       <c r="T23" s="9" t="s">
-        <v>70</v>
+        <v>25</v>
       </c>
       <c r="V23" s="6"/>
       <c r="W23" s="6"/>
@@ -4257,33 +3148,42 @@
       <c r="AD23" s="6"/>
     </row>
     <row r="24" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B24" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" s="4"/>
-      <c r="F24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="J24" s="6"/>
-      <c r="L24" s="6"/>
-      <c r="N24" s="6"/>
-      <c r="P24" s="6"/>
-      <c r="R24" s="6"/>
-      <c r="T24" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="V24" s="6"/>
-      <c r="W24" s="6"/>
-      <c r="X24" s="6"/>
-      <c r="Y24" s="6"/>
-      <c r="Z24" s="6"/>
-      <c r="AA24" s="6"/>
-      <c r="AB24" s="6"/>
-      <c r="AC24" s="6"/>
-      <c r="AD24" s="6"/>
+      <c r="A24" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
+      <c r="R24" s="2"/>
+      <c r="S24" s="2"/>
+      <c r="T24" s="2"/>
+      <c r="U24" s="2"/>
+      <c r="V24" s="2"/>
+      <c r="W24" s="2"/>
+      <c r="X24" s="2"/>
+      <c r="Y24" s="2"/>
+      <c r="Z24" s="2"/>
+      <c r="AA24" s="2"/>
+      <c r="AB24" s="2"/>
+      <c r="AC24" s="2"/>
+      <c r="AD24" s="2"/>
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B25" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C25" s="4"/>
       <c r="F25" s="6"/>
@@ -4294,7 +3194,7 @@
       <c r="P25" s="6"/>
       <c r="R25" s="6"/>
       <c r="T25" s="9" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="V25" s="6"/>
       <c r="W25" s="6"/>
@@ -4308,7 +3208,7 @@
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B26" s="5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C26" s="4"/>
       <c r="F26" s="6"/>
@@ -4316,10 +3216,12 @@
       <c r="J26" s="6"/>
       <c r="L26" s="6"/>
       <c r="N26" s="6"/>
-      <c r="P26" s="6"/>
+      <c r="P26" s="9" t="s">
+        <v>68</v>
+      </c>
       <c r="R26" s="6"/>
       <c r="T26" s="9" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="V26" s="6"/>
       <c r="W26" s="6"/>
@@ -4333,7 +3235,7 @@
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B27" s="5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C27" s="4"/>
       <c r="F27" s="6"/>
@@ -4341,10 +3243,12 @@
       <c r="J27" s="6"/>
       <c r="L27" s="6"/>
       <c r="N27" s="6"/>
-      <c r="P27" s="6"/>
+      <c r="P27" s="9" t="s">
+        <v>68</v>
+      </c>
       <c r="R27" s="6"/>
       <c r="T27" s="9" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="V27" s="6"/>
       <c r="W27" s="6"/>
@@ -4358,7 +3262,7 @@
     </row>
     <row r="28" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B28" s="5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C28" s="4"/>
       <c r="F28" s="6"/>
@@ -4366,10 +3270,12 @@
       <c r="J28" s="6"/>
       <c r="L28" s="6"/>
       <c r="N28" s="6"/>
-      <c r="P28" s="6"/>
+      <c r="P28" s="9" t="s">
+        <v>67</v>
+      </c>
       <c r="R28" s="6"/>
       <c r="T28" s="9" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="V28" s="6"/>
       <c r="W28" s="6"/>
@@ -4382,506 +3288,36 @@
       <c r="AD28" s="6"/>
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B29" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C29" s="4"/>
-      <c r="F29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="J29" s="6"/>
-      <c r="L29" s="6"/>
-      <c r="N29" s="6"/>
-      <c r="P29" s="6"/>
-      <c r="R29" s="6"/>
-      <c r="T29" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="V29" s="6"/>
-      <c r="W29" s="6"/>
-      <c r="X29" s="6"/>
-      <c r="Y29" s="6"/>
-      <c r="Z29" s="6"/>
-      <c r="AA29" s="6"/>
-      <c r="AB29" s="6"/>
-      <c r="AC29" s="6"/>
-      <c r="AD29" s="6"/>
-    </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B30" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C30" s="4"/>
-      <c r="F30" s="6"/>
-      <c r="H30" s="6"/>
-      <c r="J30" s="6"/>
-      <c r="L30" s="6"/>
-      <c r="N30" s="6"/>
-      <c r="P30" s="6"/>
-      <c r="R30" s="6"/>
-      <c r="T30" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="V30" s="6"/>
-      <c r="W30" s="6"/>
-      <c r="X30" s="6"/>
-      <c r="Y30" s="6"/>
-      <c r="Z30" s="6"/>
-      <c r="AA30" s="6"/>
-      <c r="AB30" s="6"/>
-      <c r="AC30" s="6"/>
-      <c r="AD30" s="6"/>
-    </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-      <c r="L31" s="2"/>
-      <c r="M31" s="2"/>
-      <c r="N31" s="2"/>
-      <c r="O31" s="2"/>
-      <c r="P31" s="2"/>
-      <c r="Q31" s="2"/>
-      <c r="R31" s="2"/>
-      <c r="S31" s="2"/>
-      <c r="T31" s="2"/>
-      <c r="U31" s="2"/>
-      <c r="V31" s="2"/>
-      <c r="W31" s="2"/>
-      <c r="X31" s="2"/>
-      <c r="Y31" s="2"/>
-      <c r="Z31" s="2"/>
-      <c r="AA31" s="2"/>
-      <c r="AB31" s="2"/>
-      <c r="AC31" s="2"/>
-      <c r="AD31" s="2"/>
-    </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B32" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C32" s="4"/>
-      <c r="F32" s="6"/>
-      <c r="H32" s="6"/>
-      <c r="J32" s="6"/>
-      <c r="L32" s="6"/>
-      <c r="N32" s="6"/>
-      <c r="P32" s="6"/>
-      <c r="R32" s="6"/>
-      <c r="T32" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="V32" s="6"/>
-      <c r="W32" s="6"/>
-      <c r="X32" s="6"/>
-      <c r="Y32" s="6"/>
-      <c r="Z32" s="6"/>
-      <c r="AA32" s="6"/>
-      <c r="AB32" s="6"/>
-      <c r="AC32" s="6"/>
-      <c r="AD32" s="6"/>
-    </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B33" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C33" s="4"/>
-      <c r="F33" s="6"/>
-      <c r="H33" s="6"/>
-      <c r="J33" s="6"/>
-      <c r="L33" s="6"/>
-      <c r="N33" s="6"/>
-      <c r="P33" s="6"/>
-      <c r="R33" s="6"/>
-      <c r="T33" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="V33" s="6"/>
-      <c r="W33" s="6"/>
-      <c r="X33" s="6"/>
-      <c r="Y33" s="6"/>
-      <c r="Z33" s="6"/>
-      <c r="AA33" s="6"/>
-      <c r="AB33" s="6"/>
-      <c r="AC33" s="6"/>
-      <c r="AD33" s="6"/>
-    </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B34" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C34" s="4"/>
-      <c r="F34" s="6"/>
-      <c r="H34" s="6"/>
-      <c r="J34" s="6"/>
-      <c r="L34" s="6"/>
-      <c r="N34" s="6"/>
-      <c r="P34" s="6"/>
-      <c r="R34" s="6"/>
-      <c r="T34" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="V34" s="6"/>
-      <c r="W34" s="6"/>
-      <c r="X34" s="6"/>
-      <c r="Y34" s="6"/>
-      <c r="Z34" s="6"/>
-      <c r="AA34" s="6"/>
-      <c r="AB34" s="6"/>
-      <c r="AC34" s="6"/>
-      <c r="AD34" s="6"/>
-    </row>
-    <row r="35" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B35" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C35" s="4"/>
-      <c r="F35" s="6"/>
-      <c r="H35" s="6"/>
-      <c r="J35" s="6"/>
-      <c r="L35" s="6"/>
-      <c r="N35" s="6"/>
-      <c r="P35" s="6"/>
-      <c r="R35" s="6"/>
-      <c r="T35" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="V35" s="6"/>
-      <c r="W35" s="6"/>
-      <c r="X35" s="6"/>
-      <c r="Y35" s="6"/>
-      <c r="Z35" s="6"/>
-      <c r="AA35" s="6"/>
-      <c r="AB35" s="6"/>
-      <c r="AC35" s="6"/>
-      <c r="AD35" s="6"/>
-    </row>
-    <row r="36" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B36" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C36" s="4"/>
-      <c r="F36" s="6"/>
-      <c r="H36" s="6"/>
-      <c r="J36" s="6"/>
-      <c r="L36" s="6"/>
-      <c r="N36" s="6"/>
-      <c r="P36" s="6"/>
-      <c r="R36" s="6"/>
-      <c r="T36" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="V36" s="6"/>
-      <c r="W36" s="6"/>
-      <c r="X36" s="6"/>
-      <c r="Y36" s="6"/>
-      <c r="Z36" s="6"/>
-      <c r="AA36" s="6"/>
-      <c r="AB36" s="6"/>
-      <c r="AC36" s="6"/>
-      <c r="AD36" s="6"/>
-    </row>
-    <row r="37" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
-      <c r="I37" s="2"/>
-      <c r="J37" s="2"/>
-      <c r="K37" s="2"/>
-      <c r="L37" s="2"/>
-      <c r="M37" s="2"/>
-      <c r="N37" s="2"/>
-      <c r="O37" s="2"/>
-      <c r="P37" s="2"/>
-      <c r="Q37" s="2"/>
-      <c r="R37" s="2"/>
-      <c r="S37" s="2"/>
-      <c r="T37" s="2"/>
-      <c r="U37" s="2"/>
-      <c r="V37" s="2"/>
-      <c r="W37" s="2"/>
-      <c r="X37" s="2"/>
-      <c r="Y37" s="2"/>
-      <c r="Z37" s="2"/>
-      <c r="AA37" s="2"/>
-      <c r="AB37" s="2"/>
-      <c r="AC37" s="2"/>
-      <c r="AD37" s="2"/>
-    </row>
-    <row r="38" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B38" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C38" s="4"/>
-      <c r="F38" s="6"/>
-      <c r="H38" s="6"/>
-      <c r="J38" s="6"/>
-      <c r="L38" s="6"/>
-      <c r="N38" s="6"/>
-      <c r="P38" s="6"/>
-      <c r="R38" s="6"/>
-      <c r="T38" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="V38" s="6"/>
-      <c r="W38" s="6"/>
-      <c r="X38" s="6"/>
-      <c r="Y38" s="6"/>
-      <c r="Z38" s="6"/>
-      <c r="AA38" s="6"/>
-      <c r="AB38" s="6"/>
-      <c r="AC38" s="6"/>
-      <c r="AD38" s="6"/>
-    </row>
-    <row r="39" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B39" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C39" s="4"/>
-      <c r="F39" s="6"/>
-      <c r="H39" s="6"/>
-      <c r="J39" s="6"/>
-      <c r="L39" s="6"/>
-      <c r="N39" s="6"/>
-      <c r="P39" s="6"/>
-      <c r="R39" s="6"/>
-      <c r="T39" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="V39" s="6"/>
-      <c r="W39" s="6"/>
-      <c r="X39" s="6"/>
-      <c r="Y39" s="6"/>
-      <c r="Z39" s="6"/>
-      <c r="AA39" s="6"/>
-      <c r="AB39" s="6"/>
-      <c r="AC39" s="6"/>
-      <c r="AD39" s="6"/>
-    </row>
-    <row r="40" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B40" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C40" s="4"/>
-      <c r="F40" s="6"/>
-      <c r="H40" s="6"/>
-      <c r="J40" s="6"/>
-      <c r="L40" s="6"/>
-      <c r="N40" s="6"/>
-      <c r="P40" s="6"/>
-      <c r="R40" s="6"/>
-      <c r="T40" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="V40" s="6"/>
-      <c r="W40" s="6"/>
-      <c r="X40" s="6"/>
-      <c r="Y40" s="6"/>
-      <c r="Z40" s="6"/>
-      <c r="AA40" s="6"/>
-      <c r="AB40" s="6"/>
-      <c r="AC40" s="6"/>
-      <c r="AD40" s="6"/>
-    </row>
-    <row r="41" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B41" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C41" s="4"/>
-      <c r="F41" s="6"/>
-      <c r="H41" s="6"/>
-      <c r="J41" s="6"/>
-      <c r="L41" s="6"/>
-      <c r="N41" s="6"/>
-      <c r="P41" s="6"/>
-      <c r="R41" s="6"/>
-      <c r="T41" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="V41" s="6"/>
-      <c r="W41" s="6"/>
-      <c r="X41" s="6"/>
-      <c r="Y41" s="6"/>
-      <c r="Z41" s="6"/>
-      <c r="AA41" s="6"/>
-      <c r="AB41" s="6"/>
-      <c r="AC41" s="6"/>
-      <c r="AD41" s="6"/>
-    </row>
-    <row r="42" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B42" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C42" s="4"/>
-      <c r="F42" s="6"/>
-      <c r="H42" s="6"/>
-      <c r="J42" s="6"/>
-      <c r="L42" s="6"/>
-      <c r="N42" s="6"/>
-      <c r="P42" s="6"/>
-      <c r="R42" s="6"/>
-      <c r="T42" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="V42" s="6"/>
-      <c r="W42" s="6"/>
-      <c r="X42" s="6"/>
-      <c r="Y42" s="6"/>
-      <c r="Z42" s="6"/>
-      <c r="AA42" s="6"/>
-      <c r="AB42" s="6"/>
-      <c r="AC42" s="6"/>
-      <c r="AD42" s="6"/>
-    </row>
-    <row r="43" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A43" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
-      <c r="H43" s="2"/>
-      <c r="I43" s="2"/>
-      <c r="J43" s="2"/>
-      <c r="K43" s="2"/>
-      <c r="L43" s="2"/>
-      <c r="M43" s="2"/>
-      <c r="N43" s="2"/>
-      <c r="O43" s="2"/>
-      <c r="P43" s="2"/>
-      <c r="Q43" s="2"/>
-      <c r="R43" s="2"/>
-      <c r="S43" s="2"/>
-      <c r="T43" s="2"/>
-      <c r="U43" s="2"/>
-      <c r="V43" s="2"/>
-      <c r="W43" s="2"/>
-      <c r="X43" s="2"/>
-      <c r="Y43" s="2"/>
-      <c r="Z43" s="2"/>
-      <c r="AA43" s="2"/>
-      <c r="AB43" s="2"/>
-      <c r="AC43" s="2"/>
-      <c r="AD43" s="2"/>
-    </row>
-    <row r="44" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B44" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C44" s="4"/>
-      <c r="F44" s="6"/>
-      <c r="H44" s="6"/>
-      <c r="J44" s="6"/>
-      <c r="L44" s="6"/>
-      <c r="N44" s="6"/>
-      <c r="P44" s="6"/>
-      <c r="R44" s="6"/>
-      <c r="T44" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="V44" s="6"/>
-      <c r="W44" s="6"/>
-      <c r="X44" s="6"/>
-      <c r="Y44" s="6"/>
-      <c r="Z44" s="6"/>
-      <c r="AA44" s="6"/>
-      <c r="AB44" s="6"/>
-      <c r="AC44" s="6"/>
-      <c r="AD44" s="6"/>
-    </row>
-    <row r="45" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B45" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C45" s="4"/>
-      <c r="F45" s="6"/>
-      <c r="H45" s="6"/>
-      <c r="J45" s="6"/>
-      <c r="L45" s="6"/>
-      <c r="N45" s="6"/>
-      <c r="P45" s="6"/>
-      <c r="R45" s="6"/>
-      <c r="T45" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="V45" s="6"/>
-      <c r="W45" s="6"/>
-      <c r="X45" s="6"/>
-      <c r="Y45" s="6"/>
-      <c r="Z45" s="6"/>
-      <c r="AA45" s="6"/>
-      <c r="AB45" s="6"/>
-      <c r="AC45" s="6"/>
-      <c r="AD45" s="6"/>
-    </row>
-    <row r="46" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B46" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C46" s="4"/>
-      <c r="F46" s="6"/>
-      <c r="H46" s="6"/>
-      <c r="J46" s="6"/>
-      <c r="L46" s="6"/>
-      <c r="N46" s="6"/>
-      <c r="P46" s="6"/>
-      <c r="R46" s="6"/>
-      <c r="T46" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="V46" s="6"/>
-      <c r="W46" s="6"/>
-      <c r="X46" s="6"/>
-      <c r="Y46" s="6"/>
-      <c r="Z46" s="6"/>
-      <c r="AA46" s="6"/>
-      <c r="AB46" s="6"/>
-      <c r="AC46" s="6"/>
-      <c r="AD46" s="6"/>
-    </row>
-    <row r="47" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B47" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C47" s="4"/>
-      <c r="F47" s="6"/>
-      <c r="H47" s="6"/>
-      <c r="J47" s="6"/>
-      <c r="L47" s="6"/>
-      <c r="N47" s="6"/>
-      <c r="P47" s="6"/>
-      <c r="R47" s="6"/>
-      <c r="T47" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="V47" s="6"/>
-      <c r="W47" s="6"/>
-      <c r="X47" s="6"/>
-      <c r="Y47" s="6"/>
-      <c r="Z47" s="6"/>
-      <c r="AA47" s="6"/>
-      <c r="AB47" s="6"/>
-      <c r="AC47" s="6"/>
-      <c r="AD47" s="6"/>
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
+      <c r="P29" s="3"/>
+      <c r="Q29" s="3"/>
+      <c r="R29" s="3"/>
+      <c r="S29" s="3"/>
+      <c r="T29" s="3"/>
+      <c r="U29" s="3"/>
+      <c r="V29" s="3"/>
+      <c r="W29" s="3"/>
+      <c r="X29" s="3"/>
+      <c r="Y29" s="3"/>
+      <c r="Z29" s="3"/>
+      <c r="AA29" s="3"/>
+      <c r="AB29" s="3"/>
+      <c r="AC29" s="3"/>
+      <c r="AD29" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4980,29 +3416,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1032" r:id="rId7" name="Check Box 8">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>13</xdr:col>
-                    <xdr:colOff>228600</xdr:colOff>
-                    <xdr:row>6</xdr:row>
-                    <xdr:rowOff>114300</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>13</xdr:col>
-                    <xdr:colOff>584200</xdr:colOff>
-                    <xdr:row>8</xdr:row>
-                    <xdr:rowOff>12700</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1033" r:id="rId8" name="Check Box 9">
+            <control shapeId="1033" r:id="rId7" name="Check Box 9">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -5024,7 +3438,51 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1034" r:id="rId9" name="Check Box 10">
+            <control shapeId="1034" r:id="rId8" name="Check Box 10">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>13</xdr:col>
+                    <xdr:colOff>228600</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>114300</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>13</xdr:col>
+                    <xdr:colOff>584200</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>12700</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1035" r:id="rId9" name="Check Box 11">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>13</xdr:col>
+                    <xdr:colOff>228600</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>114300</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>13</xdr:col>
+                    <xdr:colOff>584200</xdr:colOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>12700</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1036" r:id="rId10" name="Check Box 12">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -5046,29 +3504,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1035" r:id="rId10" name="Check Box 11">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>13</xdr:col>
-                    <xdr:colOff>228600</xdr:colOff>
-                    <xdr:row>10</xdr:row>
-                    <xdr:rowOff>114300</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>13</xdr:col>
-                    <xdr:colOff>584200</xdr:colOff>
-                    <xdr:row>12</xdr:row>
-                    <xdr:rowOff>12700</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1036" r:id="rId11" name="Check Box 12">
+            <control shapeId="1038" r:id="rId11" name="Check Box 14">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -5090,19 +3526,19 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1037" r:id="rId12" name="Check Box 13">
+            <control shapeId="1039" r:id="rId12" name="Check Box 15">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>13</xdr:col>
                     <xdr:colOff>228600</xdr:colOff>
-                    <xdr:row>12</xdr:row>
+                    <xdr:row>11</xdr:row>
                     <xdr:rowOff>114300</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>13</xdr:col>
                     <xdr:colOff>584200</xdr:colOff>
-                    <xdr:row>14</xdr:row>
+                    <xdr:row>13</xdr:row>
                     <xdr:rowOff>12700</xdr:rowOff>
                   </to>
                 </anchor>
@@ -5112,7 +3548,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1038" r:id="rId13" name="Check Box 14">
+            <control shapeId="1041" r:id="rId13" name="Check Box 17">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -5134,19 +3570,19 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1039" r:id="rId14" name="Check Box 15">
+            <control shapeId="1042" r:id="rId14" name="Check Box 18">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>13</xdr:col>
                     <xdr:colOff>228600</xdr:colOff>
-                    <xdr:row>15</xdr:row>
+                    <xdr:row>14</xdr:row>
                     <xdr:rowOff>114300</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>13</xdr:col>
                     <xdr:colOff>584200</xdr:colOff>
-                    <xdr:row>17</xdr:row>
+                    <xdr:row>16</xdr:row>
                     <xdr:rowOff>12700</xdr:rowOff>
                   </to>
                 </anchor>
@@ -5156,29 +3592,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1040" r:id="rId15" name="Check Box 16">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>13</xdr:col>
-                    <xdr:colOff>228600</xdr:colOff>
-                    <xdr:row>16</xdr:row>
-                    <xdr:rowOff>114300</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>13</xdr:col>
-                    <xdr:colOff>584200</xdr:colOff>
-                    <xdr:row>18</xdr:row>
-                    <xdr:rowOff>12700</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1041" r:id="rId16" name="Check Box 17">
+            <control shapeId="1052" r:id="rId15" name="Check Box 28">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -5200,7 +3614,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1042" r:id="rId17" name="Check Box 18">
+            <control shapeId="1053" r:id="rId16" name="Check Box 29">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -5222,7 +3636,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1043" r:id="rId18" name="Check Box 19">
+            <control shapeId="1054" r:id="rId17" name="Check Box 30">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -5244,7 +3658,29 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1044" r:id="rId19" name="Check Box 20">
+            <control shapeId="1055" r:id="rId18" name="Check Box 31">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>13</xdr:col>
+                    <xdr:colOff>228600</xdr:colOff>
+                    <xdr:row>20</xdr:row>
+                    <xdr:rowOff>114300</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>13</xdr:col>
+                    <xdr:colOff>584200</xdr:colOff>
+                    <xdr:row>22</xdr:row>
+                    <xdr:rowOff>12700</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1056" r:id="rId19" name="Check Box 32">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -5266,29 +3702,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1045" r:id="rId20" name="Check Box 21">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>13</xdr:col>
-                    <xdr:colOff>228600</xdr:colOff>
-                    <xdr:row>22</xdr:row>
-                    <xdr:rowOff>114300</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>13</xdr:col>
-                    <xdr:colOff>584200</xdr:colOff>
-                    <xdr:row>24</xdr:row>
-                    <xdr:rowOff>12700</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1046" r:id="rId21" name="Check Box 22">
+            <control shapeId="1057" r:id="rId20" name="Check Box 33">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -5310,7 +3724,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1047" r:id="rId22" name="Check Box 23">
+            <control shapeId="1058" r:id="rId21" name="Check Box 34">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -5332,7 +3746,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1048" r:id="rId23" name="Check Box 24">
+            <control shapeId="1059" r:id="rId22" name="Check Box 35">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -5354,7 +3768,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1049" r:id="rId24" name="Check Box 25">
+            <control shapeId="1060" r:id="rId23" name="Check Box 36">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -5376,359 +3790,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1050" r:id="rId25" name="Check Box 26">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>13</xdr:col>
-                    <xdr:colOff>228600</xdr:colOff>
-                    <xdr:row>27</xdr:row>
-                    <xdr:rowOff>114300</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>13</xdr:col>
-                    <xdr:colOff>584200</xdr:colOff>
-                    <xdr:row>29</xdr:row>
-                    <xdr:rowOff>12700</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1051" r:id="rId26" name="Check Box 27">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>13</xdr:col>
-                    <xdr:colOff>228600</xdr:colOff>
-                    <xdr:row>28</xdr:row>
-                    <xdr:rowOff>114300</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>13</xdr:col>
-                    <xdr:colOff>584200</xdr:colOff>
-                    <xdr:row>30</xdr:row>
-                    <xdr:rowOff>12700</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1052" r:id="rId27" name="Check Box 28">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>13</xdr:col>
-                    <xdr:colOff>228600</xdr:colOff>
-                    <xdr:row>30</xdr:row>
-                    <xdr:rowOff>114300</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>13</xdr:col>
-                    <xdr:colOff>584200</xdr:colOff>
-                    <xdr:row>32</xdr:row>
-                    <xdr:rowOff>12700</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1053" r:id="rId28" name="Check Box 29">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>13</xdr:col>
-                    <xdr:colOff>228600</xdr:colOff>
-                    <xdr:row>31</xdr:row>
-                    <xdr:rowOff>114300</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>13</xdr:col>
-                    <xdr:colOff>584200</xdr:colOff>
-                    <xdr:row>33</xdr:row>
-                    <xdr:rowOff>12700</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1054" r:id="rId29" name="Check Box 30">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>13</xdr:col>
-                    <xdr:colOff>228600</xdr:colOff>
-                    <xdr:row>32</xdr:row>
-                    <xdr:rowOff>114300</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>13</xdr:col>
-                    <xdr:colOff>584200</xdr:colOff>
-                    <xdr:row>34</xdr:row>
-                    <xdr:rowOff>12700</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1055" r:id="rId30" name="Check Box 31">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>13</xdr:col>
-                    <xdr:colOff>228600</xdr:colOff>
-                    <xdr:row>33</xdr:row>
-                    <xdr:rowOff>114300</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>13</xdr:col>
-                    <xdr:colOff>584200</xdr:colOff>
-                    <xdr:row>35</xdr:row>
-                    <xdr:rowOff>12700</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1056" r:id="rId31" name="Check Box 32">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>13</xdr:col>
-                    <xdr:colOff>228600</xdr:colOff>
-                    <xdr:row>34</xdr:row>
-                    <xdr:rowOff>114300</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>13</xdr:col>
-                    <xdr:colOff>584200</xdr:colOff>
-                    <xdr:row>36</xdr:row>
-                    <xdr:rowOff>12700</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1057" r:id="rId32" name="Check Box 33">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>13</xdr:col>
-                    <xdr:colOff>228600</xdr:colOff>
-                    <xdr:row>36</xdr:row>
-                    <xdr:rowOff>114300</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>13</xdr:col>
-                    <xdr:colOff>584200</xdr:colOff>
-                    <xdr:row>38</xdr:row>
-                    <xdr:rowOff>12700</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1058" r:id="rId33" name="Check Box 34">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>13</xdr:col>
-                    <xdr:colOff>228600</xdr:colOff>
-                    <xdr:row>37</xdr:row>
-                    <xdr:rowOff>114300</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>13</xdr:col>
-                    <xdr:colOff>584200</xdr:colOff>
-                    <xdr:row>39</xdr:row>
-                    <xdr:rowOff>12700</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1059" r:id="rId34" name="Check Box 35">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>13</xdr:col>
-                    <xdr:colOff>228600</xdr:colOff>
-                    <xdr:row>38</xdr:row>
-                    <xdr:rowOff>114300</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>13</xdr:col>
-                    <xdr:colOff>584200</xdr:colOff>
-                    <xdr:row>40</xdr:row>
-                    <xdr:rowOff>12700</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1060" r:id="rId35" name="Check Box 36">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>13</xdr:col>
-                    <xdr:colOff>228600</xdr:colOff>
-                    <xdr:row>39</xdr:row>
-                    <xdr:rowOff>114300</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>13</xdr:col>
-                    <xdr:colOff>584200</xdr:colOff>
-                    <xdr:row>41</xdr:row>
-                    <xdr:rowOff>12700</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1061" r:id="rId36" name="Check Box 37">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>13</xdr:col>
-                    <xdr:colOff>228600</xdr:colOff>
-                    <xdr:row>40</xdr:row>
-                    <xdr:rowOff>114300</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>13</xdr:col>
-                    <xdr:colOff>584200</xdr:colOff>
-                    <xdr:row>42</xdr:row>
-                    <xdr:rowOff>12700</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1062" r:id="rId37" name="Check Box 38">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>13</xdr:col>
-                    <xdr:colOff>228600</xdr:colOff>
-                    <xdr:row>42</xdr:row>
-                    <xdr:rowOff>114300</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>13</xdr:col>
-                    <xdr:colOff>584200</xdr:colOff>
-                    <xdr:row>44</xdr:row>
-                    <xdr:rowOff>12700</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1063" r:id="rId38" name="Check Box 39">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>13</xdr:col>
-                    <xdr:colOff>228600</xdr:colOff>
-                    <xdr:row>43</xdr:row>
-                    <xdr:rowOff>114300</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>13</xdr:col>
-                    <xdr:colOff>584200</xdr:colOff>
-                    <xdr:row>45</xdr:row>
-                    <xdr:rowOff>12700</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1064" r:id="rId39" name="Check Box 40">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>13</xdr:col>
-                    <xdr:colOff>228600</xdr:colOff>
-                    <xdr:row>44</xdr:row>
-                    <xdr:rowOff>114300</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>13</xdr:col>
-                    <xdr:colOff>584200</xdr:colOff>
-                    <xdr:row>46</xdr:row>
-                    <xdr:rowOff>12700</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1065" r:id="rId40" name="Check Box 41">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>13</xdr:col>
-                    <xdr:colOff>228600</xdr:colOff>
-                    <xdr:row>45</xdr:row>
-                    <xdr:rowOff>114300</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>13</xdr:col>
-                    <xdr:colOff>584200</xdr:colOff>
-                    <xdr:row>47</xdr:row>
-                    <xdr:rowOff>12700</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1066" r:id="rId41" name="Check Box 42">
+            <control shapeId="1066" r:id="rId24" name="Check Box 42">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -5748,6 +3810,50 @@
             </control>
           </mc:Choice>
         </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1067" r:id="rId25" name="Check Box 43">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>13</xdr:col>
+                    <xdr:colOff>228600</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>114300</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>13</xdr:col>
+                    <xdr:colOff>584200</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>12700</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1068" r:id="rId26" name="Check Box 44">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>13</xdr:col>
+                    <xdr:colOff>228600</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>114300</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>13</xdr:col>
+                    <xdr:colOff>584200</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>12700</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
       </controls>
     </mc:Choice>
   </mc:AlternateContent>
@@ -5758,15 +3864,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66F8186B-541E-CB41-B7D3-31AE7BE22136}">
   <dimension ref="A1:O58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:15" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="17" thickTop="1" x14ac:dyDescent="0.2">
@@ -5786,30 +3892,30 @@
     </row>
     <row r="3" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="F4" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="H4" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="J4" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="L4" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="N4" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -5850,11 +3956,11 @@
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
       <c r="H6" s="12" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="I6" s="11"/>
       <c r="J6" s="18" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
       <c r="K6" s="10"/>
       <c r="L6" s="11"/>
@@ -5872,7 +3978,7 @@
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
       <c r="J7" s="18" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="K7" s="10"/>
       <c r="L7" s="11"/>
@@ -5980,7 +4086,7 @@
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
       <c r="H12" s="11" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="I12" s="11"/>
       <c r="J12" s="10"/>
@@ -5998,7 +4104,7 @@
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
       <c r="H13" s="11" t="s">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="I13" s="11"/>
       <c r="J13" s="10"/>
@@ -6072,7 +4178,7 @@
     </row>
     <row r="18" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B18" s="14" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="2:15" ht="17" thickTop="1" x14ac:dyDescent="0.2">
@@ -6175,7 +4281,7 @@
       <c r="F23" s="16"/>
       <c r="G23" s="16"/>
       <c r="H23" s="17" t="s">
-        <v>86</v>
+        <v>57</v>
       </c>
       <c r="I23" s="15"/>
       <c r="J23" s="16"/>
@@ -6193,7 +4299,7 @@
       <c r="F24" s="16"/>
       <c r="G24" s="16"/>
       <c r="H24" s="17" t="s">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="I24" s="15"/>
       <c r="J24" s="16"/>
@@ -6241,7 +4347,7 @@
       <c r="F26" s="15"/>
       <c r="G26" s="15"/>
       <c r="H26" s="28" t="s">
-        <v>87</v>
+        <v>58</v>
       </c>
       <c r="I26" s="16"/>
       <c r="J26" s="15"/>
@@ -6259,7 +4365,7 @@
       <c r="F27" s="15"/>
       <c r="G27" s="15"/>
       <c r="H27" s="28" t="s">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="I27" s="16"/>
       <c r="J27" s="15"/>
@@ -6307,7 +4413,7 @@
       <c r="F29" s="16"/>
       <c r="G29" s="16"/>
       <c r="H29" s="17" t="s">
-        <v>88</v>
+        <v>59</v>
       </c>
       <c r="I29" s="15"/>
       <c r="J29" s="16"/>
@@ -6325,7 +4431,7 @@
       <c r="F30" s="16"/>
       <c r="G30" s="16"/>
       <c r="H30" s="17" t="s">
-        <v>52</v>
+        <v>77</v>
       </c>
       <c r="I30" s="15"/>
       <c r="J30" s="16"/>
@@ -6367,7 +4473,7 @@
     </row>
     <row r="35" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B35" s="19" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="2:15" ht="17" thickTop="1" x14ac:dyDescent="0.2">
@@ -6408,7 +4514,7 @@
       <c r="F37" s="20"/>
       <c r="G37" s="20"/>
       <c r="H37" s="26" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="I37" s="21"/>
       <c r="J37" s="20"/>
@@ -6425,9 +4531,7 @@
       <c r="E38" s="21"/>
       <c r="F38" s="20"/>
       <c r="G38" s="20"/>
-      <c r="H38" s="26" t="s">
-        <v>90</v>
-      </c>
+      <c r="H38" s="26"/>
       <c r="I38" s="21"/>
       <c r="J38" s="20"/>
       <c r="K38" s="20"/>
@@ -6474,7 +4578,7 @@
       <c r="F40" s="21"/>
       <c r="G40" s="21"/>
       <c r="H40" s="27" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="I40" s="20"/>
       <c r="J40" s="21"/>
@@ -6492,7 +4596,7 @@
       <c r="F41" s="21"/>
       <c r="G41" s="21"/>
       <c r="H41" s="27" t="s">
-        <v>92</v>
+        <v>60</v>
       </c>
       <c r="I41" s="20"/>
       <c r="J41" s="21"/>
@@ -6539,9 +4643,7 @@
       <c r="E43" s="21"/>
       <c r="F43" s="20"/>
       <c r="G43" s="20"/>
-      <c r="H43" s="26" t="s">
-        <v>83</v>
-      </c>
+      <c r="H43" s="26"/>
       <c r="I43" s="21"/>
       <c r="J43" s="20"/>
       <c r="K43" s="20"/>
@@ -6557,9 +4659,7 @@
       <c r="E44" s="21"/>
       <c r="F44" s="20"/>
       <c r="G44" s="20"/>
-      <c r="H44" s="26" t="s">
-        <v>84</v>
-      </c>
+      <c r="H44" s="26"/>
       <c r="I44" s="21"/>
       <c r="J44" s="20"/>
       <c r="K44" s="20"/>
@@ -6606,7 +4706,7 @@
       <c r="F46" s="21"/>
       <c r="G46" s="21"/>
       <c r="H46" s="27" t="s">
-        <v>79</v>
+        <v>52</v>
       </c>
       <c r="I46" s="20"/>
       <c r="J46" s="21"/>
@@ -6624,7 +4724,7 @@
       <c r="F47" s="21"/>
       <c r="G47" s="21"/>
       <c r="H47" s="27" t="s">
-        <v>80</v>
+        <v>53</v>
       </c>
       <c r="I47" s="20"/>
       <c r="J47" s="21"/>
@@ -6658,7 +4758,7 @@
     </row>
     <row r="52" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B52" s="22" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
     </row>
     <row r="53" spans="2:15" ht="17" thickTop="1" x14ac:dyDescent="0.2">
@@ -6699,7 +4799,7 @@
       <c r="F54" s="23"/>
       <c r="G54" s="23"/>
       <c r="H54" s="25" t="s">
-        <v>81</v>
+        <v>54</v>
       </c>
       <c r="I54" s="24"/>
       <c r="J54" s="23"/>
@@ -6745,7 +4845,7 @@
       <c r="D57" s="23"/>
       <c r="E57" s="23"/>
       <c r="F57" s="25" t="s">
-        <v>85</v>
+        <v>56</v>
       </c>
       <c r="G57" s="24"/>
     </row>
@@ -6774,17 +4874,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>